<commit_message>
16.11.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/Others/IMEI.xlsx
+++ b/Others/IMEI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DC0723-D83F-48FE-B704-556227350DEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A170466C-5A7B-48CC-A8AE-85150DBE9C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="960" windowWidth="10845" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
   <si>
     <t>D40</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>B12+</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>s40</t>
   </si>
 </sst>
 </file>
@@ -373,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -425,6 +431,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>357653104891481</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>359998100004623</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>359998100271040</v>
@@ -449,12 +471,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>355580101577908</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="15" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>356243107327526</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>358444100265204</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
17.11.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/Others/IMEI.xlsx
+++ b/Others/IMEI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A170466C-5A7B-48CC-A8AE-85150DBE9C88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD7F4B8-AF5F-4A57-8D45-E2683168808C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="510" windowWidth="11910" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t>D40</t>
   </si>
@@ -463,14 +463,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>359998100056409</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="13" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>355580101577908</v>

</xml_diff>

<commit_message>
18.11.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/Others/IMEI.xlsx
+++ b/Others/IMEI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD7F4B8-AF5F-4A57-8D45-E2683168808C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFA3EC4-5F18-42CB-876F-3F50C43B9123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="510" windowWidth="11910" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>D40</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>s40</t>
+  </si>
+  <si>
+    <t>i97</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Doa Mosjid Market</t>
+  </si>
+  <si>
+    <t>Doa Mobile Park</t>
   </si>
 </sst>
 </file>
@@ -79,7 +91,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,16 +99,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -379,19 +412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="3" max="3" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>357653103198649</v>
       </c>
@@ -399,7 +433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>357653103196023</v>
       </c>
@@ -407,7 +441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>357653103005687</v>
       </c>
@@ -415,76 +449,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>357653103200007</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>357653103200007</v>
+        <v>357653102912248</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>357653102912248</v>
+        <v>357653104891481</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>357653104891481</v>
+        <v>359998100004623</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>359998100004623</v>
+        <v>359998100271040</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>359998100271040</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>359998100048380</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>355580101577908</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="C12" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>356243107327526</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>358444100265204</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>357261101684444</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
24.11.19 & 25.11.19 Sales Details
</commit_message>
<xml_diff>
--- a/Others/IMEI.xlsx
+++ b/Others/IMEI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFA3EC4-5F18-42CB-876F-3F50C43B9123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ABB34B-E32F-4561-988B-3C382C159ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>D40</t>
   </si>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -481,14 +481,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>359998100271040</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
     <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>355580101577908</v>

</xml_diff>

<commit_message>
03.12.19 MC Sales Details
</commit_message>
<xml_diff>
--- a/Others/IMEI.xlsx
+++ b/Others/IMEI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29ABB34B-E32F-4561-988B-3C382C159ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D5D87E-022A-41EB-8EC3-612D250F3BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>D40</t>
   </si>
@@ -412,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -425,14 +425,6 @@
     <col min="3" max="3" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>357653103198649</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="2" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>357653103196023</v>

</xml_diff>